<commit_message>
Update pathway analysis of pro only p-value less than 0.05.xlsx
</commit_message>
<xml_diff>
--- a/Pathway analysis/Second pathway analysis only using p-value/pathway analysis of pro only p-value less than 0.05.xlsx
+++ b/Pathway analysis/Second pathway analysis only using p-value/pathway analysis of pro only p-value less than 0.05.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sabde\OneDrive\Documents\UM documents\BMS Year 3\Internship + Thesis\Sabrina_BMS_Bachelor-Internship\Pathway analysis\Second pathway analysis only using p-value\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F03CA726-0583-4FE4-8D9F-F7712676F457}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9C5846-CB06-441D-AAC9-8877A2225164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="9490" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pathway analysis of pro only p-" sheetId="1" r:id="rId1"/>
@@ -1819,7 +1819,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2655,11 +2655,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G590"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>